<commit_message>
modificación de calculos de costos fijos
</commit_message>
<xml_diff>
--- a/T3/Pauta tablas T2.xlsx
+++ b/T3/Pauta tablas T2.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoYera\Desktop\2025-2\Econo_Med\Tareas_Economed\T3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368EB603-9E30-4AFB-94D5-A5418960D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19995" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="preg1-Norma" sheetId="6" r:id="rId1"/>
     <sheet name="preg2-Optima" sheetId="5" r:id="rId2"/>
     <sheet name="preg1 sin politica" sheetId="7" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -423,7 +442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -503,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -522,18 +541,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -545,10 +557,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -609,7 +621,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPr id="3" name="2 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -657,19 +675,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>256444</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>4397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>255467</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>57639</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPr id="3" name="2 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -689,8 +713,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="24460200"/>
-          <a:ext cx="5619750" cy="1708150"/>
+          <a:off x="256444" y="23772935"/>
+          <a:ext cx="5611446" cy="1665166"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -713,9 +737,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -753,7 +777,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -825,7 +849,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,11 +1022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N151"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141:C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1591,11 +1615,11 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="30">
+      <c r="F25" s="27">
         <f>+SUM(F3:F24)</f>
         <v>66428.939999999988</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="27">
         <f>+SUM(G3:G24)</f>
         <v>15059.48</v>
       </c>
@@ -1644,19 +1668,19 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="31" t="s">
         <v>122</v>
       </c>
       <c r="G29" s="2"/>
@@ -1707,8 +1731,8 @@
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="6" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1889,7 @@
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="2"/>
@@ -1925,19 +1949,19 @@
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="26">
+      <c r="C50" s="24"/>
+      <c r="D50" s="23">
         <v>0.5</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="28" t="s">
+      <c r="G50" s="25" t="s">
         <v>111</v>
       </c>
       <c r="H50" s="2"/>
@@ -1947,7 +1971,7 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="28" t="s">
+      <c r="G51" s="25" t="s">
         <v>112</v>
       </c>
       <c r="H51" s="2"/>
@@ -1961,14 +1985,14 @@
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="24"/>
-      <c r="J53" s="23"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="21"/>
+      <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
@@ -1994,37 +2018,37 @@
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="H56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I56" s="11" t="s">
+      <c r="I56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J56" s="11" t="s">
+      <c r="J56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="K56" s="11" t="s">
+      <c r="K56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="L56" s="11" t="s">
+      <c r="L56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="11" t="s">
+      <c r="M56" s="10" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2032,50 +2056,50 @@
       <c r="A57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D57" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G57" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="I57" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="13" t="s">
+      <c r="J57" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="L57" s="13" t="s">
+      <c r="L57" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="M57" s="15" t="s">
+      <c r="M57" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C58" s="11"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="11"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -2084,18 +2108,18 @@
       <c r="B59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17" t="s">
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F59" s="17">
+      <c r="F59" s="14">
         <f>+VLOOKUP($B59,$C$16:$G$21,5,0)</f>
         <v>439</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -2108,16 +2132,16 @@
       <c r="B60" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17">
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14">
         <f>+VLOOKUP($B60,$C$9:$G$15,5,0)</f>
         <v>169</v>
       </c>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -2130,21 +2154,21 @@
       <c r="B61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="17">
+      <c r="C61" s="14">
         <f>+G5</f>
         <v>575</v>
       </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17" t="s">
+      <c r="D61" s="14"/>
+      <c r="E61" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="14">
         <f>+VLOOKUP($B61,$C$16:$G$21,5,0)</f>
         <v>58</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
       <c r="J61" s="2">
         <f>+G24</f>
         <v>200</v>
@@ -2160,16 +2184,16 @@
       <c r="B62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17">
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14">
         <f>+VLOOKUP($B62,$C$16:$G$21,5,0)</f>
         <v>97</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -2182,16 +2206,16 @@
       <c r="B63" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17">
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14">
         <f>+VLOOKUP($B63,$C$9:$G$15,5,0)</f>
         <v>203</v>
       </c>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17">
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14">
         <f>+G23</f>
         <v>192</v>
       </c>
@@ -2207,22 +2231,22 @@
       <c r="B64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="14">
         <f>+G6</f>
         <v>1664.48</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="14">
         <f>+G8</f>
         <v>731</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="14">
         <f>+VLOOKUP($B64,$C$9:$G$15,5,0)</f>
         <v>700</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -2232,19 +2256,19 @@
       <c r="A65" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17">
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14">
         <f>+VLOOKUP($B65,$C$16:$G$21,5,0)</f>
         <v>71</v>
       </c>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -2257,19 +2281,19 @@
       <c r="B66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17">
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14">
         <f>+VLOOKUP($B66,$C$9:$G$16,5,0)</f>
         <v>233.44</v>
       </c>
-      <c r="F66" s="17">
+      <c r="F66" s="14">
         <f>+VLOOKUP($B66,$C$16:$G$21,5,0)</f>
         <v>134.56</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -2282,21 +2306,21 @@
       <c r="B67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17" t="s">
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="17">
+      <c r="F67" s="14">
         <f>+VLOOKUP($B67,$C$16:$G$21,5,0)</f>
         <v>134</v>
       </c>
-      <c r="G67" s="17">
+      <c r="G67" s="14">
         <f>+G3</f>
         <v>60</v>
       </c>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -2309,18 +2333,18 @@
       <c r="B68" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="14">
         <f>+G7</f>
         <v>806</v>
       </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17" t="s">
+      <c r="D68" s="14"/>
+      <c r="E68" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
@@ -2333,18 +2357,18 @@
       <c r="B69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17">
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14">
         <f>+VLOOKUP($B69,$C$9:$G$15,5,0)</f>
         <v>1043</v>
       </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17">
+      <c r="F69" s="14"/>
+      <c r="G69" s="14">
         <f>+G4</f>
         <v>204</v>
       </c>
-      <c r="H69" s="17">
+      <c r="H69" s="14">
         <f>+G22</f>
         <v>7071</v>
       </c>
@@ -2361,16 +2385,16 @@
       <c r="B70" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17">
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14">
         <f>+VLOOKUP($B70,$C$9:$G$15,5,0)</f>
         <v>135</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -2383,16 +2407,16 @@
       <c r="B71" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17">
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14">
         <f>+VLOOKUP($B71,$C$9:$G$15,5,0)</f>
         <v>139</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -2483,36 +2507,36 @@
       <c r="A76" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="17"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="23"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="20"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="17"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="14"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B78" s="11"/>
+      <c r="B78" s="10"/>
       <c r="C78" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E78" s="16"/>
-      <c r="F78" s="17"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -2521,24 +2545,24 @@
       <c r="A79" t="s">
         <v>51</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F79" s="17"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="13"/>
+      <c r="B80" s="12"/>
       <c r="C80" s="7">
         <v>2030</v>
       </c>
@@ -2548,7 +2572,7 @@
       <c r="E80" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F80" s="17"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -2557,20 +2581,20 @@
       <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="17">
+      <c r="B81" s="13"/>
+      <c r="C81" s="14">
         <f>+'preg1 sin politica'!D81</f>
         <v>264</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="14">
         <f t="shared" ref="D81:D87" si="3">+G35</f>
         <v>264</v>
       </c>
-      <c r="E81" s="19">
+      <c r="E81" s="16">
         <f t="shared" ref="E81:E87" si="4">+D81/C81-1</f>
         <v>0</v>
       </c>
-      <c r="F81" s="17"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -2579,20 +2603,20 @@
       <c r="A82" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="17">
+      <c r="B82" s="13"/>
+      <c r="C82" s="14">
         <f>+'preg1 sin politica'!D82</f>
         <v>4774.84</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="14">
         <f t="shared" si="3"/>
         <v>3045.48</v>
       </c>
-      <c r="E82" s="19">
+      <c r="E82" s="16">
         <f t="shared" si="4"/>
         <v>-0.36218176944148917</v>
       </c>
-      <c r="F82" s="17"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -2601,20 +2625,20 @@
       <c r="A83" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="17">
+      <c r="B83" s="13"/>
+      <c r="C83" s="14">
         <f>+'preg1 sin politica'!D83</f>
         <v>731</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="14">
         <f t="shared" si="3"/>
         <v>731</v>
       </c>
-      <c r="E83" s="19">
+      <c r="E83" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F83" s="17"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2623,20 +2647,20 @@
       <c r="A84" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="11"/>
-      <c r="C84" s="17">
+      <c r="B84" s="10"/>
+      <c r="C84" s="14">
         <f>+'preg1 sin politica'!D84</f>
         <v>3556</v>
       </c>
-      <c r="D84" s="17">
+      <c r="D84" s="14">
         <f t="shared" si="3"/>
         <v>3556</v>
       </c>
-      <c r="E84" s="19">
+      <c r="E84" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F84" s="17"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -2645,20 +2669,20 @@
       <c r="A85" t="s">
         <v>45</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="17">
+      <c r="B85" s="10"/>
+      <c r="C85" s="14">
         <f>+'preg1 sin politica'!D85</f>
         <v>5571</v>
       </c>
-      <c r="D85" s="17">
+      <c r="D85" s="14">
         <f t="shared" si="3"/>
         <v>7071</v>
       </c>
-      <c r="E85" s="19">
+      <c r="E85" s="16">
         <f t="shared" si="4"/>
         <v>0.26925148088314477</v>
       </c>
-      <c r="F85" s="17"/>
+      <c r="F85" s="14"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -2667,20 +2691,20 @@
       <c r="A86" t="s">
         <v>46</v>
       </c>
-      <c r="B86" s="11"/>
-      <c r="C86" s="17">
+      <c r="B86" s="10"/>
+      <c r="C86" s="14">
         <f>+'preg1 sin politica'!D86</f>
         <v>192</v>
       </c>
-      <c r="D86" s="17">
+      <c r="D86" s="14">
         <f t="shared" si="3"/>
         <v>192</v>
       </c>
-      <c r="E86" s="19">
+      <c r="E86" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F86" s="17"/>
+      <c r="F86" s="14"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2689,20 +2713,20 @@
       <c r="A87" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="11"/>
-      <c r="C87" s="17">
+      <c r="B87" s="10"/>
+      <c r="C87" s="14">
         <f>+'preg1 sin politica'!D87</f>
         <v>200</v>
       </c>
-      <c r="D87" s="17">
+      <c r="D87" s="14">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="E87" s="19">
+      <c r="E87" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F87" s="17"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2711,11 +2735,11 @@
       <c r="A88" t="s">
         <v>48</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="16"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2724,11 +2748,11 @@
       <c r="A89" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -2737,11 +2761,11 @@
       <c r="A90" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="17"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="14"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -2784,49 +2808,49 @@
       <c r="A94" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="24"/>
-      <c r="I94" s="24"/>
-      <c r="J94" s="23"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="20"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="11"/>
+      <c r="B96" s="10"/>
       <c r="C96" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E96" s="11"/>
+      <c r="E96" s="10"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B97" s="11"/>
-      <c r="C97" s="11" t="s">
+      <c r="B97" s="10"/>
+      <c r="C97" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D97" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="13" t="s">
         <v>24</v>
       </c>
       <c r="F97" s="2"/>
@@ -2836,7 +2860,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
-      <c r="B98" s="13"/>
+      <c r="B98" s="12"/>
       <c r="C98" s="7">
         <v>2030</v>
       </c>
@@ -2855,21 +2879,21 @@
       <c r="A99" t="s">
         <v>28</v>
       </c>
-      <c r="B99" s="11"/>
-      <c r="C99" s="17">
+      <c r="B99" s="10"/>
+      <c r="C99" s="14">
         <f>+'preg1 sin politica'!D99</f>
         <v>1271.6399999999999</v>
       </c>
-      <c r="D99" s="17">
+      <c r="D99" s="14">
         <f t="shared" ref="D99:D104" si="5">+F35</f>
         <v>1271.6399999999999</v>
       </c>
-      <c r="E99" s="19">
+      <c r="E99" s="16">
         <f t="shared" ref="E99:E104" si="6">+D99/C99-1</f>
         <v>0</v>
       </c>
       <c r="F99" s="2"/>
-      <c r="G99" s="22" t="s">
+      <c r="G99" s="19" t="s">
         <v>54</v>
       </c>
       <c r="H99" s="2"/>
@@ -2879,16 +2903,16 @@
       <c r="A100" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="11"/>
-      <c r="C100" s="17">
+      <c r="B100" s="10"/>
+      <c r="C100" s="14">
         <f>+'preg1 sin politica'!D100</f>
         <v>32183.24</v>
       </c>
-      <c r="D100" s="17">
+      <c r="D100" s="14">
         <f t="shared" si="5"/>
         <v>20971.149999999998</v>
       </c>
-      <c r="E100" s="19">
+      <c r="E100" s="16">
         <f t="shared" si="6"/>
         <v>-0.34838288500474168</v>
       </c>
@@ -2901,16 +2925,16 @@
       <c r="A101" t="s">
         <v>37</v>
       </c>
-      <c r="B101" s="11"/>
-      <c r="C101" s="17">
+      <c r="B101" s="10"/>
+      <c r="C101" s="14">
         <f>+'preg1 sin politica'!D101</f>
         <v>815.8</v>
       </c>
-      <c r="D101" s="17">
+      <c r="D101" s="14">
         <f t="shared" si="5"/>
         <v>3397.68</v>
       </c>
-      <c r="E101" s="19">
+      <c r="E101" s="16">
         <f t="shared" si="6"/>
         <v>3.1648443245893603</v>
       </c>
@@ -2925,16 +2949,16 @@
       <c r="A102" t="s">
         <v>38</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="17">
+      <c r="B102" s="10"/>
+      <c r="C102" s="14">
         <f>+'preg1 sin politica'!D102</f>
         <v>2018.6</v>
       </c>
-      <c r="D102" s="17">
+      <c r="D102" s="14">
         <f t="shared" si="5"/>
         <v>2764.8100000000004</v>
       </c>
-      <c r="E102" s="19">
+      <c r="E102" s="16">
         <f t="shared" si="6"/>
         <v>0.36966709600713399</v>
       </c>
@@ -2947,16 +2971,16 @@
       <c r="A103" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="17">
+      <c r="B103" s="10"/>
+      <c r="C103" s="14">
         <f>+'preg1 sin politica'!D103</f>
         <v>29281.18</v>
       </c>
-      <c r="D103" s="17">
+      <c r="D103" s="14">
         <f t="shared" si="5"/>
         <v>37165.18</v>
       </c>
-      <c r="E103" s="19">
+      <c r="E103" s="16">
         <f t="shared" si="6"/>
         <v>0.26925144410163804</v>
       </c>
@@ -2969,16 +2993,16 @@
       <c r="A104" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="11"/>
-      <c r="C104" s="17">
+      <c r="B104" s="10"/>
+      <c r="C104" s="14">
         <f>+'preg1 sin politica'!D104</f>
         <v>420.48</v>
       </c>
-      <c r="D104" s="17">
+      <c r="D104" s="14">
         <f t="shared" si="5"/>
         <v>420.48</v>
       </c>
-      <c r="E104" s="19">
+      <c r="E104" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2991,16 +3015,16 @@
       <c r="A105" t="s">
         <v>47</v>
       </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="17">
+      <c r="B105" s="10"/>
+      <c r="C105" s="14">
         <f>+'preg1 sin politica'!D105</f>
         <v>438</v>
       </c>
-      <c r="D105" s="17">
+      <c r="D105" s="14">
         <f t="shared" ref="D105" si="7">+F41</f>
         <v>438</v>
       </c>
-      <c r="E105" s="19">
+      <c r="E105" s="16">
         <f t="shared" ref="E105" si="8">+D105/C105-1</f>
         <v>0</v>
       </c>
@@ -3013,10 +3037,10 @@
       <c r="A106" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="11"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -3026,10 +3050,10 @@
       <c r="A107" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -3039,20 +3063,20 @@
       <c r="A108" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -3062,16 +3086,16 @@
       <c r="A110" t="s">
         <v>52</v>
       </c>
-      <c r="B110" s="11"/>
-      <c r="C110" s="17">
+      <c r="B110" s="10"/>
+      <c r="C110" s="14">
         <f>+SUM(C99:C108)</f>
         <v>66428.94</v>
       </c>
-      <c r="D110" s="17">
+      <c r="D110" s="14">
         <f>+SUM(D99:D108)</f>
         <v>66428.939999999988</v>
       </c>
-      <c r="E110" s="17"/>
+      <c r="E110" s="14"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -3089,32 +3113,32 @@
       <c r="A113" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E113" s="11"/>
-      <c r="H113" s="24"/>
-      <c r="I113" s="24"/>
-      <c r="J113" s="23"/>
+      <c r="E113" s="10"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+      <c r="J113" s="20"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E114" s="11"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C115" s="35"/>
-      <c r="E115" s="11"/>
+      <c r="C115" s="32"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E116" s="11"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
@@ -3129,13 +3153,13 @@
       <c r="D117" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E117" s="11"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>54</v>
       </c>
-      <c r="E118" s="11"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -3149,61 +3173,61 @@
         <f>+E30/1000000</f>
         <v>2293.6289000000002</v>
       </c>
-      <c r="D119" s="19">
+      <c r="D119" s="16">
         <f>+C119/B119-1</f>
         <v>0.2622094914470372</v>
       </c>
-      <c r="E119" s="11"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
-      <c r="E120" s="11"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E123" s="11"/>
-      <c r="H123" s="24"/>
-      <c r="I123" s="24"/>
-      <c r="J123" s="23"/>
+      <c r="E123" s="10"/>
+      <c r="H123" s="21"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="20"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E124" s="11"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C125" s="35"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="32"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E126" s="11"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
@@ -3218,13 +3242,13 @@
       <c r="D127" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E127" s="11"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>54</v>
       </c>
-      <c r="E128" s="11"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -3238,11 +3262,11 @@
         <f>+C119+SUM(A30:C30)/1000000</f>
         <v>2466.6682137900002</v>
       </c>
-      <c r="D129" s="19">
+      <c r="D129" s="16">
         <f>+C129/B129-1</f>
         <v>-0.1529996471024575</v>
       </c>
-      <c r="E129" s="11"/>
+      <c r="E129" s="10"/>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
@@ -3250,49 +3274,49 @@
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
-      <c r="E130" s="11"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E133" s="11"/>
-      <c r="H133" s="24"/>
-      <c r="I133" s="24"/>
-      <c r="J133" s="23"/>
+      <c r="E133" s="10"/>
+      <c r="H133" s="21"/>
+      <c r="I133" s="21"/>
+      <c r="J133" s="20"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E134" s="11"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E135" s="11"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B136" s="11" t="s">
+      <c r="B136" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E136" s="11"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="6"/>
@@ -3305,7 +3329,7 @@
       <c r="D137" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E137" s="11"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -3319,14 +3343,14 @@
         <f>+A28*1000</f>
         <v>2490</v>
       </c>
-      <c r="D138" s="19">
+      <c r="D138" s="16">
         <f>+C138/B138-1</f>
         <v>-0.99017712730285223</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G138" s="21" t="s">
+      <c r="G138" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3342,11 +3366,11 @@
         <f>+B28*1000</f>
         <v>22290</v>
       </c>
-      <c r="D139" s="19">
+      <c r="D139" s="16">
         <f>+C139/B139-1</f>
         <v>-0.9068026926453987</v>
       </c>
-      <c r="E139" s="11"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
@@ -3360,14 +3384,14 @@
         <f>+C28*1000</f>
         <v>94240</v>
       </c>
-      <c r="D140" s="19">
+      <c r="D140" s="16">
         <f>+C140/B140-1</f>
         <v>-4.6732753388630366E-2</v>
       </c>
-      <c r="E140" s="11"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A141" s="14" t="s">
+      <c r="A141" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B141" s="2">
@@ -3378,75 +3402,75 @@
         <f>+D28*1000</f>
         <v>20496430</v>
       </c>
-      <c r="D141" s="19">
+      <c r="D141" s="16">
         <f>+C141/B141-1</f>
         <v>-0.24574322688241923</v>
       </c>
-      <c r="E141" s="11"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
-      <c r="E142" s="11"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3462,11 +3486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4473,11 +4497,11 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="30">
+      <c r="F25" s="27">
         <f>+SUM(F3:F24)</f>
         <v>66428.95</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="27">
         <f>+SUM(G3:G24)</f>
         <v>15288.84</v>
       </c>
@@ -4502,7 +4526,7 @@
       <c r="C27" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>75</v>
       </c>
       <c r="E27" s="2"/>
@@ -4531,19 +4555,19 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="31" t="s">
         <v>121</v>
       </c>
       <c r="F29" s="2"/>
@@ -4600,8 +4624,8 @@
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="6" t="s">
         <v>4</v>
       </c>
@@ -4751,7 +4775,7 @@
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="2"/>
@@ -4811,20 +4835,20 @@
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="26">
+      <c r="C50" s="24"/>
+      <c r="D50" s="23">
         <v>0.5</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="28" t="s">
+      <c r="H50" s="25" t="s">
         <v>111</v>
       </c>
       <c r="I50" s="2"/>
@@ -4834,7 +4858,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="28" t="s">
+      <c r="H51" s="25" t="s">
         <v>112</v>
       </c>
       <c r="I51" s="2"/>
@@ -4843,22 +4867,22 @@
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="24"/>
-      <c r="J53" s="23"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="21"/>
+      <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
@@ -4884,40 +4908,40 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="33" t="s">
+      <c r="C56" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="H56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I56" s="11" t="s">
+      <c r="I56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J56" s="11" t="s">
+      <c r="J56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="K56" s="11" t="s">
+      <c r="K56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="L56" s="11" t="s">
+      <c r="L56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="11" t="s">
+      <c r="M56" s="10" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4925,68 +4949,68 @@
       <c r="A57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D57" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G57" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="I57" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="13" t="s">
+      <c r="J57" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="L57" s="13" t="s">
+      <c r="L57" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="M57" s="15" t="s">
+      <c r="M57" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B58" s="11"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="11"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>32</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14">
         <f>+VLOOKUP($R59,$C$10:$G$21,5,0)</f>
         <v>439</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -4999,17 +5023,17 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14">
         <f t="shared" ref="F60:F67" si="2">+VLOOKUP($R60,$C$10:$G$21,5,0)</f>
         <v>169</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -5022,22 +5046,22 @@
       <c r="A61" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14">
         <f>+G7</f>
         <v>575</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="14">
         <f>+G8</f>
         <v>2581.84</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="14">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
       <c r="J61" s="2">
         <f>+G24</f>
         <v>200</v>
@@ -5053,17 +5077,17 @@
       <c r="A62" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -5076,17 +5100,17 @@
       <c r="A63" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14">
         <f t="shared" si="2"/>
         <v>203</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17">
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14">
         <f>+G23</f>
         <v>192</v>
       </c>
@@ -5102,23 +5126,23 @@
       <c r="A64" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="14">
         <f>+G5</f>
         <v>812</v>
       </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17">
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14">
         <f>+G9</f>
         <v>731</v>
       </c>
-      <c r="F64" s="17">
+      <c r="F64" s="14">
         <f t="shared" si="2"/>
         <v>700</v>
       </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -5131,17 +5155,17 @@
       <c r="A65" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -5154,17 +5178,17 @@
       <c r="A66" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14">
         <f t="shared" si="2"/>
         <v>368</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -5177,20 +5201,20 @@
       <c r="A67" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="G67" s="17">
+      <c r="G67" s="14">
         <f>+G3</f>
         <v>60</v>
       </c>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -5203,19 +5227,19 @@
       <c r="A68" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="14">
         <f>+G6</f>
         <v>806</v>
       </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17" t="s">
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
@@ -5228,19 +5252,19 @@
       <c r="A69" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14">
         <f>+VLOOKUP($R69,$C$10:$G$21,5,0)</f>
         <v>1043</v>
       </c>
-      <c r="G69" s="17">
+      <c r="G69" s="14">
         <f>+G4</f>
         <v>204</v>
       </c>
-      <c r="H69" s="17">
+      <c r="H69" s="14">
         <f>+G22</f>
         <v>5571</v>
       </c>
@@ -5257,17 +5281,17 @@
       <c r="A70" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14">
         <f>+VLOOKUP($R70,$C$10:$G$21,5,0)</f>
         <v>135</v>
       </c>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -5280,17 +5304,17 @@
       <c r="A71" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17">
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14">
         <f>+VLOOKUP($R71,$C$10:$G$21,5,0)</f>
         <v>139</v>
       </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -5390,36 +5414,36 @@
       <c r="A76" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="17"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="23"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="20"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="17"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="14"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B78" s="11"/>
+      <c r="B78" s="10"/>
       <c r="C78" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E78" s="16"/>
-      <c r="F78" s="17"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -5428,24 +5452,24 @@
       <c r="A79" t="s">
         <v>51</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F79" s="17"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="13"/>
+      <c r="B80" s="12"/>
       <c r="C80" s="7">
         <v>2030</v>
       </c>
@@ -5455,7 +5479,7 @@
       <c r="E80" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F80" s="17"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -5464,20 +5488,20 @@
       <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16">
+      <c r="B81" s="13"/>
+      <c r="C81" s="13">
         <f>+'preg1-Norma'!D81</f>
         <v>264</v>
       </c>
-      <c r="D81" s="17">
+      <c r="D81" s="14">
         <f t="shared" ref="D81:D86" si="4">+G35</f>
         <v>264</v>
       </c>
-      <c r="E81" s="19">
+      <c r="E81" s="16">
         <f t="shared" ref="E81:E86" si="5">+D81/C81-1</f>
         <v>0</v>
       </c>
-      <c r="F81" s="17"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -5486,20 +5510,20 @@
       <c r="A82" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16">
+      <c r="B82" s="13"/>
+      <c r="C82" s="13">
         <f>+'preg1-Norma'!D82</f>
         <v>3045.48</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="14">
         <f t="shared" si="4"/>
         <v>4774.84</v>
       </c>
-      <c r="E82" s="19">
+      <c r="E82" s="16">
         <f t="shared" si="5"/>
         <v>0.56784480607326282</v>
       </c>
-      <c r="F82" s="17"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -5508,20 +5532,20 @@
       <c r="A83" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16">
+      <c r="B83" s="13"/>
+      <c r="C83" s="13">
         <f>+'preg1-Norma'!D83</f>
         <v>731</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="14">
         <f t="shared" si="4"/>
         <v>731</v>
       </c>
-      <c r="E83" s="19">
+      <c r="E83" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F83" s="17"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -5530,20 +5554,20 @@
       <c r="A84" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="11"/>
-      <c r="C84" s="16">
+      <c r="B84" s="10"/>
+      <c r="C84" s="13">
         <f>+'preg1-Norma'!D84</f>
         <v>3556</v>
       </c>
-      <c r="D84" s="17">
+      <c r="D84" s="14">
         <f t="shared" si="4"/>
         <v>3556</v>
       </c>
-      <c r="E84" s="19">
+      <c r="E84" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F84" s="17"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -5552,20 +5576,20 @@
       <c r="A85" t="s">
         <v>45</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="16">
+      <c r="B85" s="10"/>
+      <c r="C85" s="13">
         <f>+'preg1-Norma'!D85</f>
         <v>7071</v>
       </c>
-      <c r="D85" s="17">
+      <c r="D85" s="14">
         <f t="shared" si="4"/>
         <v>5571</v>
       </c>
-      <c r="E85" s="19">
+      <c r="E85" s="16">
         <f t="shared" si="5"/>
         <v>-0.21213406873143825</v>
       </c>
-      <c r="F85" s="17"/>
+      <c r="F85" s="14"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -5574,20 +5598,20 @@
       <c r="A86" t="s">
         <v>46</v>
       </c>
-      <c r="B86" s="11"/>
-      <c r="C86" s="16">
+      <c r="B86" s="10"/>
+      <c r="C86" s="13">
         <f>+'preg1-Norma'!D86</f>
         <v>192</v>
       </c>
-      <c r="D86" s="17">
+      <c r="D86" s="14">
         <f t="shared" si="4"/>
         <v>192</v>
       </c>
-      <c r="E86" s="19">
+      <c r="E86" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F86" s="17"/>
+      <c r="F86" s="14"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -5596,20 +5620,20 @@
       <c r="A87" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="11"/>
-      <c r="C87" s="16">
+      <c r="B87" s="10"/>
+      <c r="C87" s="13">
         <f>+'preg1-Norma'!D87</f>
         <v>200</v>
       </c>
-      <c r="D87" s="17">
+      <c r="D87" s="14">
         <f t="shared" ref="D87" si="6">+G41</f>
         <v>200</v>
       </c>
-      <c r="E87" s="19">
+      <c r="E87" s="16">
         <f t="shared" ref="E87" si="7">+D87/C87-1</f>
         <v>0</v>
       </c>
-      <c r="F87" s="17"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -5618,11 +5642,11 @@
       <c r="A88" t="s">
         <v>48</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="16"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -5631,11 +5655,11 @@
       <c r="A89" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -5644,11 +5668,11 @@
       <c r="A90" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="17"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="14"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -5691,49 +5715,49 @@
       <c r="A94" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="24"/>
-      <c r="I94" s="24"/>
-      <c r="J94" s="23"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="20"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B96" s="11"/>
+      <c r="B96" s="10"/>
       <c r="C96" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E96" s="11"/>
+      <c r="E96" s="10"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B97" s="11"/>
-      <c r="C97" s="11" t="s">
+      <c r="B97" s="10"/>
+      <c r="C97" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D97" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="13" t="s">
         <v>24</v>
       </c>
       <c r="F97" s="2"/>
@@ -5743,11 +5767,11 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13">
+      <c r="B98" s="12"/>
+      <c r="C98" s="12">
         <v>2030</v>
       </c>
-      <c r="D98" s="13">
+      <c r="D98" s="12">
         <v>2030</v>
       </c>
       <c r="E98" s="8" t="s">
@@ -5762,16 +5786,16 @@
       <c r="A99" t="s">
         <v>28</v>
       </c>
-      <c r="B99" s="11"/>
-      <c r="C99" s="17">
+      <c r="B99" s="10"/>
+      <c r="C99" s="14">
         <f>+'preg1-Norma'!D99</f>
         <v>1271.6399999999999</v>
       </c>
-      <c r="D99" s="17">
+      <c r="D99" s="14">
         <f t="shared" ref="D99:D104" si="8">+F35</f>
         <v>1271.6399999999999</v>
       </c>
-      <c r="E99" s="19">
+      <c r="E99" s="16">
         <f>+D99/C99-1</f>
         <v>0</v>
       </c>
@@ -5784,16 +5808,16 @@
       <c r="A100" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="11"/>
-      <c r="C100" s="17">
+      <c r="B100" s="10"/>
+      <c r="C100" s="14">
         <f>+'preg1-Norma'!D100</f>
         <v>20971.149999999998</v>
       </c>
-      <c r="D100" s="17">
+      <c r="D100" s="14">
         <f t="shared" si="8"/>
         <v>32183.25</v>
       </c>
-      <c r="E100" s="19">
+      <c r="E100" s="16">
         <f>+D100/C100-1</f>
         <v>0.53464402285997692</v>
       </c>
@@ -5806,16 +5830,16 @@
       <c r="A101" t="s">
         <v>37</v>
       </c>
-      <c r="B101" s="11"/>
-      <c r="C101" s="17">
+      <c r="B101" s="10"/>
+      <c r="C101" s="14">
         <f>+'preg1-Norma'!D101</f>
         <v>3397.68</v>
       </c>
-      <c r="D101" s="17">
+      <c r="D101" s="14">
         <f t="shared" si="8"/>
         <v>815.8</v>
       </c>
-      <c r="E101" s="20" t="s">
+      <c r="E101" s="17" t="s">
         <v>94</v>
       </c>
       <c r="F101" s="2"/>
@@ -5827,16 +5851,16 @@
       <c r="A102" t="s">
         <v>38</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="17">
+      <c r="B102" s="10"/>
+      <c r="C102" s="14">
         <f>+'preg1-Norma'!D102</f>
         <v>2764.8100000000004</v>
       </c>
-      <c r="D102" s="17">
+      <c r="D102" s="14">
         <f t="shared" si="8"/>
         <v>2018.6</v>
       </c>
-      <c r="E102" s="19">
+      <c r="E102" s="16">
         <f>+D102/C102-1</f>
         <v>-0.26989558052813767</v>
       </c>
@@ -5849,16 +5873,16 @@
       <c r="A103" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="17">
+      <c r="B103" s="10"/>
+      <c r="C103" s="14">
         <f>+'preg1-Norma'!D103</f>
         <v>37165.18</v>
       </c>
-      <c r="D103" s="17">
+      <c r="D103" s="14">
         <f t="shared" si="8"/>
         <v>29281.18</v>
       </c>
-      <c r="E103" s="19">
+      <c r="E103" s="16">
         <f>+D103/C103-1</f>
         <v>-0.21213404589995255</v>
       </c>
@@ -5871,16 +5895,16 @@
       <c r="A104" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="11"/>
-      <c r="C104" s="17">
+      <c r="B104" s="10"/>
+      <c r="C104" s="14">
         <f>+'preg1-Norma'!D104</f>
         <v>420.48</v>
       </c>
-      <c r="D104" s="17">
+      <c r="D104" s="14">
         <f t="shared" si="8"/>
         <v>420.48</v>
       </c>
-      <c r="E104" s="19">
+      <c r="E104" s="16">
         <f>+D104/C104-1</f>
         <v>0</v>
       </c>
@@ -5893,16 +5917,16 @@
       <c r="A105" t="s">
         <v>47</v>
       </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="17">
+      <c r="B105" s="10"/>
+      <c r="C105" s="14">
         <f>+'preg1-Norma'!D105</f>
         <v>438</v>
       </c>
-      <c r="D105" s="17">
+      <c r="D105" s="14">
         <f t="shared" ref="D105" si="9">+F41</f>
         <v>438</v>
       </c>
-      <c r="E105" s="19">
+      <c r="E105" s="16">
         <f>+D105/C105-1</f>
         <v>0</v>
       </c>
@@ -5915,10 +5939,10 @@
       <c r="A106" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -5928,10 +5952,10 @@
       <c r="A107" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -5941,20 +5965,20 @@
       <c r="A108" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -5964,16 +5988,16 @@
       <c r="A110" t="s">
         <v>52</v>
       </c>
-      <c r="B110" s="11"/>
-      <c r="C110" s="17">
+      <c r="B110" s="10"/>
+      <c r="C110" s="14">
         <f>+SUM(C99:C108)</f>
         <v>66428.939999999988</v>
       </c>
-      <c r="D110" s="17">
+      <c r="D110" s="14">
         <f>+SUM(D99:D108)</f>
         <v>66428.95</v>
       </c>
-      <c r="E110" s="17"/>
+      <c r="E110" s="14"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -5991,32 +6015,32 @@
       <c r="A113" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E113" s="11"/>
-      <c r="H113" s="24"/>
-      <c r="I113" s="24"/>
-      <c r="J113" s="23"/>
+      <c r="E113" s="10"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+      <c r="J113" s="20"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E114" s="11"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C115" s="35"/>
-      <c r="E115" s="11"/>
+      <c r="C115" s="32"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C116" s="10" t="s">
         <v>82</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E116" s="11"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
@@ -6031,13 +6055,13 @@
       <c r="D117" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E117" s="11"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>54</v>
       </c>
-      <c r="E118" s="11"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -6051,61 +6075,61 @@
         <f>+C129-SUM(A30:D30)/1000000</f>
         <v>2054.55857423</v>
       </c>
-      <c r="D119" s="19">
+      <c r="D119" s="16">
         <f>+C119/B119-1</f>
         <v>-0.10423234803590076</v>
       </c>
-      <c r="E119" s="11"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
-      <c r="E120" s="11"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E123" s="11"/>
-      <c r="H123" s="24"/>
-      <c r="I123" s="24"/>
-      <c r="J123" s="23"/>
+      <c r="E123" s="10"/>
+      <c r="H123" s="21"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="20"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E124" s="11"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C125" s="35"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="32"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C126" s="10" t="s">
         <v>82</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E126" s="11"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
@@ -6120,13 +6144,13 @@
       <c r="D127" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E127" s="11"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>54</v>
       </c>
-      <c r="E128" s="11"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -6140,73 +6164,73 @@
         <f>+E30/1000000</f>
         <v>2160.3134</v>
       </c>
-      <c r="D129" s="19">
+      <c r="D129" s="16">
         <f>+C129/B129-1</f>
         <v>-0.12419781958404952</v>
       </c>
-      <c r="E129" s="11"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
-      <c r="E130" s="11"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E133" s="11"/>
-      <c r="H133" s="24"/>
-      <c r="I133" s="24"/>
-      <c r="J133" s="23"/>
+      <c r="E133" s="10"/>
+      <c r="H133" s="21"/>
+      <c r="I133" s="21"/>
+      <c r="J133" s="20"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E134" s="11"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E135" s="11"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B136" s="11" t="s">
+      <c r="B136" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="10" t="s">
         <v>82</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E136" s="11"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="6"/>
-      <c r="B137" s="13">
+      <c r="B137" s="12">
         <v>2030</v>
       </c>
-      <c r="C137" s="13">
+      <c r="C137" s="12">
         <v>2030</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E137" s="11"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -6220,7 +6244,7 @@
         <f>+A28*1000</f>
         <v>66430</v>
       </c>
-      <c r="D138" s="19">
+      <c r="D138" s="16">
         <f>+C138/B138-1</f>
         <v>25.678714859437751</v>
       </c>
@@ -6238,11 +6262,8 @@
         <f>+B28*1000</f>
         <v>180770</v>
       </c>
-      <c r="D139" s="19">
-        <f>+C139/B139-1</f>
-        <v>7.109914759982054</v>
-      </c>
-      <c r="E139" s="11"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="10"/>
       <c r="F139" s="2"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -6257,15 +6278,15 @@
         <f>+C28*1000</f>
         <v>54250</v>
       </c>
-      <c r="D140" s="19">
+      <c r="D140" s="16">
         <f>+C140/B140-1</f>
         <v>-0.42434210526315785</v>
       </c>
-      <c r="E140" s="11"/>
+      <c r="E140" s="10"/>
       <c r="F140" s="2"/>
     </row>
     <row r="141" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A141" s="14" t="s">
+      <c r="A141" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B141" s="2">
@@ -6276,11 +6297,11 @@
         <f>+D28*1000</f>
         <v>27174050</v>
       </c>
-      <c r="D141" s="19">
+      <c r="D141" s="16">
         <f>+C141/B141-1</f>
         <v>0.32579429686047767</v>
       </c>
-      <c r="E141" s="11"/>
+      <c r="E141" s="10"/>
       <c r="F141" s="2"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
@@ -6288,64 +6309,64 @@
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
-      <c r="E142" s="11"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6360,10 +6381,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:R151"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
@@ -6902,11 +6923,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F24" s="30">
+      <c r="F24" s="27">
         <f>+SUM(F2:F23)</f>
         <v>66428.940000000017</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="27">
         <f>+SUM(G2:G23)</f>
         <v>15288.84</v>
       </c>
@@ -6941,19 +6962,19 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="31" t="s">
         <v>122</v>
       </c>
     </row>
@@ -7003,8 +7024,8 @@
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="6" t="s">
         <v>4</v>
       </c>
@@ -7134,7 +7155,7 @@
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="2"/>
@@ -7167,9 +7188,9 @@
       <c r="A52" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -7177,15 +7198,15 @@
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="11"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="10"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D54" s="2"/>
@@ -7206,36 +7227,36 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="11"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17" t="s">
+      <c r="B56" s="10"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="H56" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I56" s="11" t="s">
+      <c r="I56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J56" s="11" t="s">
+      <c r="J56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="K56" s="11" t="s">
+      <c r="K56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="L56" s="11" t="s">
+      <c r="L56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="11" t="s">
+      <c r="M56" s="10" t="s">
         <v>77</v>
       </c>
     </row>
@@ -7243,66 +7264,66 @@
       <c r="A57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F57" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G57" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H57" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="I57" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="13" t="s">
+      <c r="J57" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="L57" s="13" t="s">
+      <c r="L57" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="M57" s="15" t="s">
+      <c r="M57" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B58" s="11"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="11"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>32</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17">
+      <c r="E59" s="14"/>
+      <c r="F59" s="14">
         <f>+VLOOKUP($R59,$C$9:$G$20,5,0)</f>
         <v>439</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -7315,19 +7336,19 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17">
+      <c r="E60" s="14"/>
+      <c r="F60" s="14">
         <f t="shared" ref="F60:F71" si="2">+VLOOKUP($R60,$C$9:$G$20,5,0)</f>
         <v>169</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -7340,23 +7361,23 @@
       <c r="A61" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14">
         <f>+VLOOKUP($R61,$C$5:$G$7,5,0)</f>
         <v>575</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="14">
         <f>+G8</f>
         <v>731</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="14">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
       <c r="J61" s="2">
         <f>+G23</f>
         <v>200</v>
@@ -7372,19 +7393,19 @@
       <c r="A62" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17" t="s">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17">
+      <c r="E62" s="14"/>
+      <c r="F62" s="14">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -7397,19 +7418,19 @@
       <c r="A63" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17" t="s">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17">
+      <c r="E63" s="14"/>
+      <c r="F63" s="14">
         <f t="shared" si="2"/>
         <v>203</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17">
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14">
         <f>+G22</f>
         <v>192</v>
       </c>
@@ -7425,20 +7446,20 @@
       <c r="A64" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17">
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14">
         <f>+VLOOKUP($R64,$C$5:$G$7,5,0)</f>
         <v>3393.84</v>
       </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17">
+      <c r="E64" s="14"/>
+      <c r="F64" s="14">
         <f t="shared" si="2"/>
         <v>700</v>
       </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -7451,19 +7472,19 @@
       <c r="A65" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17" t="s">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17">
+      <c r="E65" s="14"/>
+      <c r="F65" s="14">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -7476,19 +7497,19 @@
       <c r="A66" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17" t="s">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17">
+      <c r="E66" s="14"/>
+      <c r="F66" s="14">
         <f t="shared" si="2"/>
         <v>368</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -7501,22 +7522,22 @@
       <c r="A67" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17">
+      <c r="E67" s="14"/>
+      <c r="F67" s="14">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="G67" s="17">
+      <c r="G67" s="14">
         <f>+G3</f>
         <v>60</v>
       </c>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -7529,19 +7550,19 @@
       <c r="A68" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17">
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14">
         <f>+VLOOKUP($R68,$C$5:$G$7,5,0)</f>
         <v>806</v>
       </c>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17" t="s">
+      <c r="E68" s="14"/>
+      <c r="F68" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
@@ -7554,21 +7575,21 @@
       <c r="A69" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17" t="s">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17">
+      <c r="E69" s="14"/>
+      <c r="F69" s="14">
         <f t="shared" si="2"/>
         <v>1043</v>
       </c>
-      <c r="G69" s="17">
+      <c r="G69" s="14">
         <f>+G4</f>
         <v>204</v>
       </c>
-      <c r="H69" s="17">
+      <c r="H69" s="14">
         <f>+G21</f>
         <v>5571</v>
       </c>
@@ -7585,19 +7606,19 @@
       <c r="A70" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17" t="s">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17">
+      <c r="E70" s="14"/>
+      <c r="F70" s="14">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
@@ -7610,19 +7631,19 @@
       <c r="A71" t="s">
         <v>44</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17" t="s">
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17">
+      <c r="E71" s="14"/>
+      <c r="F71" s="14">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
@@ -7700,31 +7721,31 @@
       <c r="A76" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="17"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="17"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="14"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B78" s="11"/>
+      <c r="B78" s="10"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E78" s="16"/>
-      <c r="F78" s="17"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
@@ -7732,25 +7753,25 @@
       <c r="A79" t="s">
         <v>51</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="31" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E79" s="16"/>
-      <c r="F79" s="17"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="13"/>
+      <c r="B80" s="12"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7">
         <v>2030</v>
       </c>
       <c r="E80" s="8"/>
-      <c r="F80" s="17"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
@@ -7758,14 +7779,14 @@
       <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="17">
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14">
         <f t="shared" ref="D81:D87" si="4">+G35</f>
         <v>264</v>
       </c>
-      <c r="E81" s="19"/>
-      <c r="F81" s="17"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="14"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
@@ -7773,14 +7794,14 @@
       <c r="A82" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17">
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="14">
         <f t="shared" si="4"/>
         <v>4774.84</v>
       </c>
-      <c r="E82" s="19"/>
-      <c r="F82" s="17"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="14"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
@@ -7788,14 +7809,14 @@
       <c r="A83" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="17">
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="14">
         <f t="shared" si="4"/>
         <v>731</v>
       </c>
-      <c r="E83" s="19"/>
-      <c r="F83" s="17"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="14"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
@@ -7803,14 +7824,14 @@
       <c r="A84" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="11"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="17">
+      <c r="B84" s="10"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="14">
         <f t="shared" si="4"/>
         <v>3556</v>
       </c>
-      <c r="E84" s="19"/>
-      <c r="F84" s="17"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="14"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
@@ -7818,14 +7839,14 @@
       <c r="A85" t="s">
         <v>45</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="17">
+      <c r="B85" s="10"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14">
         <f t="shared" si="4"/>
         <v>5571</v>
       </c>
-      <c r="E85" s="19"/>
-      <c r="F85" s="17"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="14"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
@@ -7833,14 +7854,14 @@
       <c r="A86" t="s">
         <v>46</v>
       </c>
-      <c r="B86" s="11"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="17">
+      <c r="B86" s="10"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="14">
         <f t="shared" si="4"/>
         <v>192</v>
       </c>
-      <c r="E86" s="19"/>
-      <c r="F86" s="17"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="14"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
@@ -7848,14 +7869,14 @@
       <c r="A87" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="11"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="17">
+      <c r="B87" s="10"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
@@ -7863,11 +7884,11 @@
       <c r="A88" t="s">
         <v>48</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="16"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
@@ -7875,11 +7896,11 @@
       <c r="A89" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
@@ -7887,11 +7908,11 @@
       <c r="A90" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="17"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="14"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
@@ -7927,49 +7948,49 @@
       <c r="A94" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="11"/>
+      <c r="B96" s="10"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E96" s="11"/>
+      <c r="E96" s="10"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11" t="s">
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E97" s="16"/>
+      <c r="E97" s="13"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
       <c r="D98" s="7">
         <v>2030</v>
       </c>
@@ -7982,13 +8003,13 @@
       <c r="A99" t="s">
         <v>28</v>
       </c>
-      <c r="B99" s="11"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17">
+      <c r="B99" s="10"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14">
         <f t="shared" ref="D99:D105" si="5">+F35</f>
         <v>1271.6399999999999</v>
       </c>
-      <c r="E99" s="19"/>
+      <c r="E99" s="16"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -7997,13 +8018,13 @@
       <c r="A100" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="11"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17">
+      <c r="B100" s="10"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14">
         <f t="shared" si="5"/>
         <v>32183.24</v>
       </c>
-      <c r="E100" s="19"/>
+      <c r="E100" s="16"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -8012,13 +8033,13 @@
       <c r="A101" t="s">
         <v>37</v>
       </c>
-      <c r="B101" s="11"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17">
+      <c r="B101" s="10"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14">
         <f t="shared" si="5"/>
         <v>815.8</v>
       </c>
-      <c r="E101" s="19"/>
+      <c r="E101" s="16"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -8027,13 +8048,13 @@
       <c r="A102" t="s">
         <v>38</v>
       </c>
-      <c r="B102" s="11"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17">
+      <c r="B102" s="10"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14">
         <f t="shared" si="5"/>
         <v>2018.6</v>
       </c>
-      <c r="E102" s="19"/>
+      <c r="E102" s="16"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -8042,13 +8063,13 @@
       <c r="A103" t="s">
         <v>45</v>
       </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17">
+      <c r="B103" s="10"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14">
         <f t="shared" si="5"/>
         <v>29281.18</v>
       </c>
-      <c r="E103" s="19"/>
+      <c r="E103" s="16"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
@@ -8057,13 +8078,13 @@
       <c r="A104" t="s">
         <v>46</v>
       </c>
-      <c r="B104" s="11"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17">
+      <c r="B104" s="10"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14">
         <f t="shared" si="5"/>
         <v>420.48</v>
       </c>
-      <c r="E104" s="19"/>
+      <c r="E104" s="16"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -8072,13 +8093,13 @@
       <c r="A105" t="s">
         <v>47</v>
       </c>
-      <c r="B105" s="11"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="17">
+      <c r="B105" s="10"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14">
         <f t="shared" si="5"/>
         <v>438</v>
       </c>
-      <c r="E105" s="17"/>
+      <c r="E105" s="14"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -8087,10 +8108,10 @@
       <c r="A106" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="11"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -8099,10 +8120,10 @@
       <c r="A107" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -8111,19 +8132,19 @@
       <c r="A108" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -8132,13 +8153,13 @@
       <c r="A110" t="s">
         <v>52</v>
       </c>
-      <c r="B110" s="11"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="17">
+      <c r="B110" s="10"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14">
         <f>+SUM(D99:D108)</f>
         <v>66428.94</v>
       </c>
-      <c r="E110" s="17"/>
+      <c r="E110" s="14"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -8154,27 +8175,27 @@
       <c r="A113" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E113" s="11"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E114" s="11"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C115" s="35"/>
-      <c r="E115" s="11"/>
+      <c r="C115" s="32"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B116" s="11"/>
-      <c r="C116" s="11" t="s">
+      <c r="B116" s="10"/>
+      <c r="C116" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E116" s="11"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
@@ -8187,13 +8208,13 @@
       <c r="D117" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E117" s="11"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>54</v>
       </c>
-      <c r="E118" s="11"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -8204,52 +8225,52 @@
         <f>+E29/1000000</f>
         <v>1817.1539</v>
       </c>
-      <c r="E119" s="11"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
-      <c r="E120" s="11"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="B122" s="10"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E123" s="11"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E124" s="11"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C125" s="35"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="32"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B126" s="11"/>
-      <c r="C126" s="11" t="s">
+      <c r="B126" s="10"/>
+      <c r="C126" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E126" s="11"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
@@ -8262,13 +8283,13 @@
       <c r="D127" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E127" s="11"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>54</v>
       </c>
-      <c r="E128" s="11"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
@@ -8279,53 +8300,53 @@
         <f>+C119+SUM(A29:C29)/1000000</f>
         <v>2912.2398891000003</v>
       </c>
-      <c r="E129" s="11"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
-      <c r="E130" s="11"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E133" s="11"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E134" s="11"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E135" s="11"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B136" s="11" t="s">
+      <c r="B136" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C136" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E136" s="11"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="6"/>
@@ -8338,7 +8359,7 @@
       <c r="D137" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E137" s="11"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -8362,7 +8383,7 @@
         <f>+B27*1000</f>
         <v>239170</v>
       </c>
-      <c r="E139" s="11"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
@@ -8373,10 +8394,10 @@
         <f>+C27*1000</f>
         <v>98860</v>
       </c>
-      <c r="E140" s="11"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A141" s="14" t="s">
+      <c r="A141" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B141" s="2"/>
@@ -8384,71 +8405,71 @@
         <f>+D27*1000</f>
         <v>27174340</v>
       </c>
-      <c r="E141" s="11"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
-      <c r="E142" s="11"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>